<commit_message>
unterstrich in reporting areas
</commit_message>
<xml_diff>
--- a/2015_Dengue_extracted.xlsx
+++ b/2015_Dengue_extracted.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Documents/GitHub/Projekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_fiona\Info\topic04_team04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9071DA1A-3733-3B4C-9CDE-150630736FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11420" yWindow="500" windowWidth="11720" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11418" yWindow="498" windowWidth="11718" windowHeight="12342"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -37,16 +36,7 @@
     <t>May</t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
     <t>Aug</t>
-  </si>
-  <si>
-    <t>Sept</t>
   </si>
   <si>
     <t>Oct</t>
@@ -597,11 +587,20 @@
   <si>
     <t>Reporting_areas</t>
   </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -695,7 +694,7 @@
         <xdr:cNvPr id="62" name="Shape 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F04563C-8096-9447-A64A-DA6D8622E44F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F04563C-8096-9447-A64A-DA6D8622E44F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -843,7 +842,7 @@
         <xdr:cNvPr id="63" name="Shape 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C661B4-C726-D343-B6C9-61C315828650}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72C661B4-C726-D343-B6C9-61C315828650}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1000,9 +999,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1040,9 +1039,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1077,7 +1076,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1112,7 +1111,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1285,22 +1284,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.3984375" customWidth="1"/>
+    <col min="1" max="1" width="28.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1317,32 +1316,32 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -1381,9 +1380,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3">
         <v>17</v>
@@ -1423,9 +1422,9 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3">
         <v>614</v>
@@ -1465,9 +1464,9 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A5" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -1506,9 +1505,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3">
         <v>6</v>
@@ -1547,9 +1546,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3">
         <v>15</v>
@@ -1589,9 +1588,9 @@
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>11</v>
@@ -1631,9 +1630,9 @@
       </c>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A9" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="3">
         <v>25</v>
@@ -1672,9 +1671,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3">
         <v>39</v>
@@ -1714,9 +1713,9 @@
       </c>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>17</v>
@@ -1756,9 +1755,9 @@
       </c>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>7</v>
@@ -1798,9 +1797,9 @@
       </c>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3">
         <v>106</v>
@@ -1840,9 +1839,9 @@
       </c>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A14" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14" s="3">
         <v>30</v>
@@ -1881,9 +1880,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A15" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
@@ -1922,9 +1921,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -1964,9 +1963,9 @@
       </c>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3">
         <v>30</v>
@@ -2006,9 +2005,9 @@
       </c>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A18" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B18" s="3">
         <v>5</v>
@@ -2047,9 +2046,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A19" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" s="3">
         <v>66</v>
@@ -2088,9 +2087,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B20" s="3">
         <v>3</v>
@@ -2130,9 +2129,9 @@
       </c>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -2172,9 +2171,9 @@
       </c>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A22" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -2213,9 +2212,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" s="3">
         <v>38</v>
@@ -2255,9 +2254,9 @@
       </c>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B24" s="3">
         <v>10</v>
@@ -2297,9 +2296,9 @@
       </c>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
@@ -2338,9 +2337,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A26" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B26" s="3">
         <v>0</v>
@@ -2379,9 +2378,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B27" s="3">
         <v>7</v>
@@ -2421,9 +2420,9 @@
       </c>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3">
         <v>126</v>
@@ -2463,9 +2462,9 @@
       </c>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B29" s="3">
         <v>5</v>
@@ -2504,9 +2503,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A30" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B30" s="3">
         <v>45</v>
@@ -2545,9 +2544,9 @@
         <v>377</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B31" s="3">
         <v>23</v>
@@ -2587,9 +2586,9 @@
       </c>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A32" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B32" s="3">
         <v>157</v>
@@ -2628,9 +2627,9 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A33" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
@@ -2670,9 +2669,9 @@
       </c>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B34" s="3">
         <v>33</v>
@@ -2711,9 +2710,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A35" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -2752,9 +2751,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A36" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B36" s="3">
         <v>0</v>
@@ -2793,9 +2792,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B37" s="3">
         <v>28</v>
@@ -2835,9 +2834,9 @@
       </c>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A38" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B38" s="3">
         <v>33</v>
@@ -2877,9 +2876,9 @@
       </c>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A39" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3">
         <v>24</v>
@@ -2919,9 +2918,9 @@
       </c>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A40" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B40" s="3">
         <v>63</v>
@@ -2960,9 +2959,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B41" s="3">
         <v>31</v>
@@ -3001,9 +3000,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A42" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B42" s="3">
         <v>40</v>
@@ -3042,9 +3041,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B43" s="3">
         <v>0</v>
@@ -3084,9 +3083,9 @@
       </c>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B44" s="3">
         <v>3</v>
@@ -3126,9 +3125,9 @@
       </c>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A45" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B45" s="3">
         <v>53</v>
@@ -3168,9 +3167,9 @@
       </c>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A46" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B46" s="3">
         <v>2</v>
@@ -3210,9 +3209,9 @@
       </c>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A47" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B47" s="3">
         <v>5</v>
@@ -3252,9 +3251,9 @@
       </c>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A48" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
@@ -3294,9 +3293,9 @@
       </c>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A49" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B49" s="3">
         <v>22</v>
@@ -3335,9 +3334,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A50" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B50" s="3">
         <v>26</v>
@@ -3377,9 +3376,9 @@
       </c>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A51" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B51" s="3">
         <v>22</v>
@@ -3419,9 +3418,9 @@
       </c>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A52" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B52" s="3">
         <v>17</v>
@@ -3460,9 +3459,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A53" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B53" s="3">
         <v>81</v>
@@ -3502,9 +3501,9 @@
       </c>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A54" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B54" s="3">
         <v>136</v>
@@ -3544,9 +3543,9 @@
       </c>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A55" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B55" s="3">
         <v>10</v>
@@ -3585,9 +3584,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A56" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B56" s="3">
         <v>10</v>
@@ -3627,9 +3626,9 @@
       </c>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A57" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
@@ -3668,9 +3667,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A58" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B58" s="3">
         <v>132</v>
@@ -3710,9 +3709,9 @@
       </c>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A59" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B59" s="3">
         <v>68</v>
@@ -3752,9 +3751,9 @@
       </c>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A60" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B60" s="3">
         <v>20</v>
@@ -3794,9 +3793,9 @@
       </c>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A61" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B61" s="3">
         <v>25</v>
@@ -3836,9 +3835,9 @@
       </c>
       <c r="N61" s="2"/>
     </row>
-    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A62" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B62" s="3">
         <v>6</v>
@@ -3877,9 +3876,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A63" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B63" s="3">
         <v>11</v>
@@ -3918,9 +3917,9 @@
         <v>392</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A64" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B64" s="3">
         <v>0</v>
@@ -3960,9 +3959,9 @@
       </c>
       <c r="N64" s="2"/>
     </row>
-    <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A65" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B65" s="3">
         <v>119</v>
@@ -4001,9 +4000,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A66" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B66" s="3">
         <v>2</v>
@@ -4043,9 +4042,9 @@
       </c>
       <c r="N66" s="2"/>
     </row>
-    <row r="67" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A67" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B67" s="3">
         <v>17</v>
@@ -4085,9 +4084,9 @@
       </c>
       <c r="N67" s="2"/>
     </row>
-    <row r="68" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A68" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B68" s="3">
         <v>37</v>
@@ -4126,9 +4125,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A69" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B69" s="3">
         <v>9</v>
@@ -4167,9 +4166,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A70" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B70" s="3">
         <v>29</v>
@@ -4209,9 +4208,9 @@
       </c>
       <c r="N70" s="2"/>
     </row>
-    <row r="71" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A71" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B71" s="3">
         <v>22</v>
@@ -4250,9 +4249,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A72" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B72" s="3">
         <v>21</v>
@@ -4292,9 +4291,9 @@
       </c>
       <c r="N72" s="2"/>
     </row>
-    <row r="73" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A73" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B73" s="3">
         <v>19</v>
@@ -4333,9 +4332,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A74" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B74" s="3">
         <v>2</v>
@@ -4374,9 +4373,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A75" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B75" s="3">
         <v>9</v>
@@ -4416,9 +4415,9 @@
       </c>
       <c r="N75" s="2"/>
     </row>
-    <row r="76" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A76" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B76" s="3">
         <v>3</v>
@@ -4458,9 +4457,9 @@
       </c>
       <c r="N76" s="2"/>
     </row>
-    <row r="77" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A77" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B77" s="3">
         <v>9</v>
@@ -4499,9 +4498,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="16.8" x14ac:dyDescent="0.65">
       <c r="A78" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B78" s="3">
         <v>9</v>
@@ -4541,7 +4540,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O78">
+  <sortState ref="A2:O78">
     <sortCondition ref="A2:A78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>